<commit_message>
OPSK-1387 NeLS sample extraction should run in "overwrite" mode
</commit_message>
<xml_diff>
--- a/test/fixtures/files/linked-samples-complete.xlsx
+++ b/test/fixtures/files/linked-samples-complete.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Sample-5</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -79,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -164,15 +171,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,6 +235,17 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>